<commit_message>
Updated Milestone 4 with David Lanter's edits
</commit_message>
<xml_diff>
--- a/assets/files/Risk_assessment_table.xlsx
+++ b/assets/files/Risk_assessment_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\ITACS_2018-08-02\Documents\ITACS_2016-08-14\Temple\ITACS\MyClasses\MIS4596_S20\04_Milestones\Milestone-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7D355F0-8DD3-8C46-B71D-E4C0E45B8B10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69979225-AC51-4614-A800-5B383C6125E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2160" yWindow="1580" windowWidth="28040" windowHeight="17440" xr2:uid="{E8543B69-8085-5245-9B11-84E091A0C761}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E8543B69-8085-5245-9B11-84E091A0C761}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Information Type</t>
   </si>
@@ -48,28 +48,55 @@
     <t>Overall Impact Rating</t>
   </si>
   <si>
-    <t>Cost Accounting/ Performance Measurement (C.3.2.7)</t>
-  </si>
-  <si>
-    <t>Collections and Receivables (C.3.2.6)</t>
-  </si>
-  <si>
-    <t>Payments (C.3.2.5)</t>
-  </si>
-  <si>
-    <t>Accounting (C.3.2.4)</t>
-  </si>
-  <si>
-    <t>Funds Control (C.3.2.3)</t>
-  </si>
-  <si>
-    <t>Reporting and Information (C.3.2.2)</t>
-  </si>
-  <si>
-    <t>Asset and Liability Management (C.3.2.1)</t>
-  </si>
-  <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>NIST SP 800-60 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset and Liability Management </t>
+  </si>
+  <si>
+    <t>C.3.2.1</t>
+  </si>
+  <si>
+    <t>Reporting and Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funds Control </t>
+  </si>
+  <si>
+    <t>C.3.2.3</t>
+  </si>
+  <si>
+    <t>Information System Categorization:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounting </t>
+  </si>
+  <si>
+    <t>C.3.2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payments </t>
+  </si>
+  <si>
+    <t>C.3.2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collections and Receivables </t>
+  </si>
+  <si>
+    <t>C.3.2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost Accounting/ Performance Measurement </t>
+  </si>
+  <si>
+    <t>C.3.2.7</t>
+  </si>
+  <si>
+    <t>C.3.2.2</t>
   </si>
 </sst>
 </file>
@@ -85,28 +112,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -129,29 +164,264 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,111 +734,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4B9749-3FCF-D549-973B-1248430D9656}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="38.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.9140625" customWidth="1"/>
+    <col min="5" max="5" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>